<commit_message>
Taint analysis results added. Still going
</commit_message>
<xml_diff>
--- a/images/AllGraphs.xlsx
+++ b/images/AllGraphs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Constraint analysis</t>
   </si>
@@ -39,6 +39,30 @@
   </si>
   <si>
     <t>Constrints vs time</t>
+  </si>
+  <si>
+    <t>PQI</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Inst</t>
+  </si>
+  <si>
+    <t>Dev</t>
+  </si>
+  <si>
+    <t>#Automated/#dev</t>
+  </si>
+  <si>
+    <t>Output comp</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>more better</t>
   </si>
 </sst>
 </file>
@@ -6116,13 +6140,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D240"/>
+  <dimension ref="A2:P248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H176" sqref="H176"/>
+    <sheetView tabSelected="1" topLeftCell="B228" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P248" sqref="P248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="17.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -7064,12 +7093,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>3.1</v>
       </c>
@@ -7084,7 +7113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>2.8</v>
       </c>
@@ -7099,7 +7128,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>2.8</v>
       </c>
@@ -7114,7 +7143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>2.7</v>
       </c>
@@ -7129,7 +7158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>3</v>
       </c>
@@ -7144,7 +7173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>3</v>
       </c>
@@ -7159,7 +7188,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>3</v>
       </c>
@@ -7173,8 +7202,20 @@
       <c r="D217">
         <v>2</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K217" t="s">
+        <v>5</v>
+      </c>
+      <c r="N217" t="s">
+        <v>12</v>
+      </c>
+      <c r="O217" t="s">
+        <v>12</v>
+      </c>
+      <c r="P217" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>2.8</v>
       </c>
@@ -7188,8 +7229,26 @@
       <c r="D218">
         <v>1</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K218" t="s">
+        <v>6</v>
+      </c>
+      <c r="L218" t="s">
+        <v>7</v>
+      </c>
+      <c r="M218" t="s">
+        <v>8</v>
+      </c>
+      <c r="N218" t="s">
+        <v>9</v>
+      </c>
+      <c r="O218" t="s">
+        <v>10</v>
+      </c>
+      <c r="P218" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>3.7</v>
       </c>
@@ -7203,8 +7262,28 @@
       <c r="D219">
         <v>2</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K219">
+        <v>129</v>
+      </c>
+      <c r="L219">
+        <v>5</v>
+      </c>
+      <c r="M219">
+        <v>8</v>
+      </c>
+      <c r="N219">
+        <f>(K219+M219)/(K219+L219)</f>
+        <v>1.0223880597014925</v>
+      </c>
+      <c r="O219">
+        <v>1</v>
+      </c>
+      <c r="P219">
+        <f xml:space="preserve"> N219 * O219</f>
+        <v>1.0223880597014925</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>3.3</v>
       </c>
@@ -7218,8 +7297,28 @@
       <c r="D220">
         <v>6</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K220">
+        <v>53</v>
+      </c>
+      <c r="L220">
+        <v>19</v>
+      </c>
+      <c r="M220">
+        <v>4</v>
+      </c>
+      <c r="N220">
+        <f t="shared" ref="N220:N248" si="1">(K220+M220)/(K220+L220)</f>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="O220">
+        <v>1</v>
+      </c>
+      <c r="P220">
+        <f xml:space="preserve"> N220 * O220</f>
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>3.1</v>
       </c>
@@ -7233,8 +7332,28 @@
       <c r="D221">
         <v>1</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K221">
+        <v>21</v>
+      </c>
+      <c r="L221">
+        <v>2</v>
+      </c>
+      <c r="M221">
+        <v>2</v>
+      </c>
+      <c r="N221">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O221">
+        <v>0.5</v>
+      </c>
+      <c r="P221">
+        <f t="shared" ref="P220:P248" si="2" xml:space="preserve"> N221 * O221</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>3.8</v>
       </c>
@@ -7248,8 +7367,28 @@
       <c r="D222">
         <v>1</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K222">
+        <v>134</v>
+      </c>
+      <c r="L222">
+        <v>4</v>
+      </c>
+      <c r="M222">
+        <v>3</v>
+      </c>
+      <c r="N222">
+        <f t="shared" si="1"/>
+        <v>0.99275362318840576</v>
+      </c>
+      <c r="O222">
+        <v>1</v>
+      </c>
+      <c r="P222">
+        <f t="shared" si="2"/>
+        <v>0.99275362318840576</v>
+      </c>
+    </row>
+    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>4.8</v>
       </c>
@@ -7263,8 +7402,28 @@
       <c r="D223">
         <v>25</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K223">
+        <v>125</v>
+      </c>
+      <c r="L223">
+        <v>1</v>
+      </c>
+      <c r="M223">
+        <v>3</v>
+      </c>
+      <c r="N223">
+        <f t="shared" si="1"/>
+        <v>1.0158730158730158</v>
+      </c>
+      <c r="O223">
+        <v>1</v>
+      </c>
+      <c r="P223">
+        <f t="shared" si="2"/>
+        <v>1.0158730158730158</v>
+      </c>
+    </row>
+    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>2.6</v>
       </c>
@@ -7278,8 +7437,28 @@
       <c r="D224">
         <v>5</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K224">
+        <v>240</v>
+      </c>
+      <c r="L224">
+        <v>8</v>
+      </c>
+      <c r="M224">
+        <v>4</v>
+      </c>
+      <c r="N224">
+        <f t="shared" si="1"/>
+        <v>0.9838709677419355</v>
+      </c>
+      <c r="O224">
+        <v>1</v>
+      </c>
+      <c r="P224">
+        <f t="shared" si="2"/>
+        <v>0.9838709677419355</v>
+      </c>
+    </row>
+    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>3.2</v>
       </c>
@@ -7293,8 +7472,28 @@
       <c r="D225">
         <v>2</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K225">
+        <v>300</v>
+      </c>
+      <c r="L225">
+        <v>2</v>
+      </c>
+      <c r="M225">
+        <v>2</v>
+      </c>
+      <c r="N225">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O225">
+        <v>1</v>
+      </c>
+      <c r="P225">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>3.4</v>
       </c>
@@ -7308,8 +7507,28 @@
       <c r="D226">
         <v>1</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K226">
+        <v>14</v>
+      </c>
+      <c r="L226">
+        <v>1</v>
+      </c>
+      <c r="M226">
+        <v>2</v>
+      </c>
+      <c r="N226">
+        <f t="shared" si="1"/>
+        <v>1.0666666666666667</v>
+      </c>
+      <c r="O226">
+        <v>1</v>
+      </c>
+      <c r="P226">
+        <f xml:space="preserve"> N226 * O226</f>
+        <v>1.0666666666666667</v>
+      </c>
+    </row>
+    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>2.8</v>
       </c>
@@ -7323,8 +7542,28 @@
       <c r="D227">
         <v>1</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K227">
+        <v>37</v>
+      </c>
+      <c r="L227">
+        <v>2</v>
+      </c>
+      <c r="M227">
+        <v>2</v>
+      </c>
+      <c r="N227">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O227">
+        <v>1</v>
+      </c>
+      <c r="P227">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>3.1</v>
       </c>
@@ -7338,8 +7577,28 @@
       <c r="D228">
         <v>2</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K228">
+        <v>40</v>
+      </c>
+      <c r="L228">
+        <v>6</v>
+      </c>
+      <c r="M228">
+        <v>4</v>
+      </c>
+      <c r="N228">
+        <f t="shared" si="1"/>
+        <v>0.95652173913043481</v>
+      </c>
+      <c r="O228">
+        <v>1</v>
+      </c>
+      <c r="P228">
+        <f xml:space="preserve"> N228 * O228</f>
+        <v>0.95652173913043481</v>
+      </c>
+    </row>
+    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>2.8</v>
       </c>
@@ -7353,8 +7612,28 @@
       <c r="D229">
         <v>1</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K229">
+        <v>50</v>
+      </c>
+      <c r="L229">
+        <v>1</v>
+      </c>
+      <c r="M229">
+        <v>3</v>
+      </c>
+      <c r="N229">
+        <f t="shared" si="1"/>
+        <v>1.0392156862745099</v>
+      </c>
+      <c r="O229">
+        <v>0.5</v>
+      </c>
+      <c r="P229">
+        <f t="shared" si="2"/>
+        <v>0.51960784313725494</v>
+      </c>
+    </row>
+    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>3.8</v>
       </c>
@@ -7367,8 +7646,28 @@
       <c r="D230">
         <v>2</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K230">
+        <v>39</v>
+      </c>
+      <c r="L230">
+        <v>1</v>
+      </c>
+      <c r="M230">
+        <v>2</v>
+      </c>
+      <c r="N230">
+        <f t="shared" si="1"/>
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="O230">
+        <v>1</v>
+      </c>
+      <c r="P230">
+        <f t="shared" si="2"/>
+        <v>1.0249999999999999</v>
+      </c>
+    </row>
+    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>3.2</v>
       </c>
@@ -7382,8 +7681,28 @@
       <c r="D231">
         <v>1</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K231">
+        <v>600</v>
+      </c>
+      <c r="L231">
+        <v>25</v>
+      </c>
+      <c r="M231">
+        <v>0</v>
+      </c>
+      <c r="N231">
+        <f t="shared" si="1"/>
+        <v>0.96</v>
+      </c>
+      <c r="O231">
+        <v>1</v>
+      </c>
+      <c r="P231">
+        <f t="shared" si="2"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>3.1</v>
       </c>
@@ -7397,8 +7716,28 @@
       <c r="D232">
         <v>1</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K232">
+        <v>35</v>
+      </c>
+      <c r="L232">
+        <v>5</v>
+      </c>
+      <c r="M232">
+        <v>20</v>
+      </c>
+      <c r="N232">
+        <f t="shared" si="1"/>
+        <v>1.375</v>
+      </c>
+      <c r="O232">
+        <v>1</v>
+      </c>
+      <c r="P232">
+        <f t="shared" si="2"/>
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>3.3</v>
       </c>
@@ -7412,8 +7751,28 @@
       <c r="D233">
         <v>1</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K233">
+        <v>61</v>
+      </c>
+      <c r="L233">
+        <v>2</v>
+      </c>
+      <c r="M233">
+        <v>3</v>
+      </c>
+      <c r="N233">
+        <f t="shared" si="1"/>
+        <v>1.0158730158730158</v>
+      </c>
+      <c r="O233">
+        <v>1</v>
+      </c>
+      <c r="P233">
+        <f t="shared" si="2"/>
+        <v>1.0158730158730158</v>
+      </c>
+    </row>
+    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>3</v>
       </c>
@@ -7427,8 +7786,28 @@
       <c r="D234">
         <v>6</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K234">
+        <v>23</v>
+      </c>
+      <c r="L234">
+        <v>1</v>
+      </c>
+      <c r="M234">
+        <v>4</v>
+      </c>
+      <c r="N234">
+        <f t="shared" si="1"/>
+        <v>1.125</v>
+      </c>
+      <c r="O234">
+        <v>1</v>
+      </c>
+      <c r="P234">
+        <f xml:space="preserve"> N234 * O234</f>
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>3.4</v>
       </c>
@@ -7442,8 +7821,28 @@
       <c r="D235">
         <v>5</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K235">
+        <v>14</v>
+      </c>
+      <c r="L235">
+        <v>1</v>
+      </c>
+      <c r="M235">
+        <v>3</v>
+      </c>
+      <c r="N235">
+        <f t="shared" si="1"/>
+        <v>1.1333333333333333</v>
+      </c>
+      <c r="O235">
+        <v>1</v>
+      </c>
+      <c r="P235">
+        <f xml:space="preserve"> N235 * O235</f>
+        <v>1.1333333333333333</v>
+      </c>
+    </row>
+    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>4.4000000000000004</v>
       </c>
@@ -7457,8 +7856,28 @@
       <c r="D236">
         <v>4</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K236">
+        <v>70</v>
+      </c>
+      <c r="L236">
+        <v>2</v>
+      </c>
+      <c r="M236">
+        <v>0</v>
+      </c>
+      <c r="N236">
+        <f t="shared" si="1"/>
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="O236">
+        <v>1</v>
+      </c>
+      <c r="P236">
+        <f t="shared" si="2"/>
+        <v>0.97222222222222221</v>
+      </c>
+    </row>
+    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>3</v>
       </c>
@@ -7472,8 +7891,28 @@
       <c r="D237">
         <v>2</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K237">
+        <v>17</v>
+      </c>
+      <c r="L237">
+        <v>1</v>
+      </c>
+      <c r="M237">
+        <v>1</v>
+      </c>
+      <c r="N237">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O237">
+        <v>1</v>
+      </c>
+      <c r="P237">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>2.9</v>
       </c>
@@ -7487,8 +7926,28 @@
       <c r="D238">
         <v>5</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K238">
+        <v>50</v>
+      </c>
+      <c r="L238">
+        <v>2</v>
+      </c>
+      <c r="M238">
+        <v>1</v>
+      </c>
+      <c r="N238">
+        <f t="shared" si="1"/>
+        <v>0.98076923076923073</v>
+      </c>
+      <c r="O238">
+        <v>1</v>
+      </c>
+      <c r="P238">
+        <f t="shared" si="2"/>
+        <v>0.98076923076923073</v>
+      </c>
+    </row>
+    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>3</v>
       </c>
@@ -7502,8 +7961,28 @@
       <c r="D239">
         <v>1</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="K239">
+        <v>90</v>
+      </c>
+      <c r="L239">
+        <v>1</v>
+      </c>
+      <c r="M239">
+        <v>2</v>
+      </c>
+      <c r="N239">
+        <f t="shared" si="1"/>
+        <v>1.0109890109890109</v>
+      </c>
+      <c r="O239">
+        <v>1</v>
+      </c>
+      <c r="P239">
+        <f t="shared" si="2"/>
+        <v>1.0109890109890109</v>
+      </c>
+    </row>
+    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>2.7</v>
       </c>
@@ -7516,6 +7995,202 @@
       </c>
       <c r="D240">
         <v>2</v>
+      </c>
+      <c r="K240">
+        <v>28</v>
+      </c>
+      <c r="L240">
+        <v>1</v>
+      </c>
+      <c r="M240">
+        <v>5</v>
+      </c>
+      <c r="N240">
+        <f t="shared" si="1"/>
+        <v>1.1379310344827587</v>
+      </c>
+      <c r="O240">
+        <v>1</v>
+      </c>
+      <c r="P240">
+        <f t="shared" si="2"/>
+        <v>1.1379310344827587</v>
+      </c>
+    </row>
+    <row r="241" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K241">
+        <v>23</v>
+      </c>
+      <c r="L241">
+        <v>1</v>
+      </c>
+      <c r="M241">
+        <v>1</v>
+      </c>
+      <c r="N241">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O241">
+        <v>1</v>
+      </c>
+      <c r="P241">
+        <f xml:space="preserve"> N241 * O241</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K242">
+        <v>58</v>
+      </c>
+      <c r="L242">
+        <v>6</v>
+      </c>
+      <c r="M242">
+        <v>4</v>
+      </c>
+      <c r="N242">
+        <f t="shared" si="1"/>
+        <v>0.96875</v>
+      </c>
+      <c r="O242">
+        <v>1</v>
+      </c>
+      <c r="P242">
+        <f t="shared" si="2"/>
+        <v>0.96875</v>
+      </c>
+    </row>
+    <row r="243" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K243">
+        <v>165</v>
+      </c>
+      <c r="L243">
+        <v>5</v>
+      </c>
+      <c r="M243">
+        <v>1</v>
+      </c>
+      <c r="N243">
+        <f t="shared" si="1"/>
+        <v>0.97647058823529409</v>
+      </c>
+      <c r="O243">
+        <v>1</v>
+      </c>
+      <c r="P243">
+        <f xml:space="preserve"> N243 * O243</f>
+        <v>0.97647058823529409</v>
+      </c>
+    </row>
+    <row r="244" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K244">
+        <v>200</v>
+      </c>
+      <c r="L244">
+        <v>4</v>
+      </c>
+      <c r="M244">
+        <v>9</v>
+      </c>
+      <c r="N244">
+        <f t="shared" si="1"/>
+        <v>1.0245098039215685</v>
+      </c>
+      <c r="O244">
+        <v>1</v>
+      </c>
+      <c r="P244">
+        <f t="shared" si="2"/>
+        <v>1.0245098039215685</v>
+      </c>
+    </row>
+    <row r="245" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K245">
+        <v>80</v>
+      </c>
+      <c r="L245">
+        <v>2</v>
+      </c>
+      <c r="M245">
+        <v>0</v>
+      </c>
+      <c r="N245">
+        <f t="shared" si="1"/>
+        <v>0.97560975609756095</v>
+      </c>
+      <c r="O245">
+        <v>1</v>
+      </c>
+      <c r="P245">
+        <f t="shared" si="2"/>
+        <v>0.97560975609756095</v>
+      </c>
+    </row>
+    <row r="246" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K246">
+        <v>71</v>
+      </c>
+      <c r="L246">
+        <v>5</v>
+      </c>
+      <c r="M246">
+        <v>2</v>
+      </c>
+      <c r="N246">
+        <f t="shared" si="1"/>
+        <v>0.96052631578947367</v>
+      </c>
+      <c r="O246">
+        <v>1</v>
+      </c>
+      <c r="P246">
+        <f t="shared" si="2"/>
+        <v>0.96052631578947367</v>
+      </c>
+    </row>
+    <row r="247" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K247">
+        <v>68</v>
+      </c>
+      <c r="L247">
+        <v>1</v>
+      </c>
+      <c r="M247">
+        <v>3</v>
+      </c>
+      <c r="N247">
+        <f t="shared" si="1"/>
+        <v>1.0289855072463767</v>
+      </c>
+      <c r="O247">
+        <v>1</v>
+      </c>
+      <c r="P247">
+        <f xml:space="preserve"> N247 * O247</f>
+        <v>1.0289855072463767</v>
+      </c>
+    </row>
+    <row r="248" spans="11:16" x14ac:dyDescent="0.25">
+      <c r="K248">
+        <v>33</v>
+      </c>
+      <c r="L248">
+        <v>2</v>
+      </c>
+      <c r="M248">
+        <v>0</v>
+      </c>
+      <c r="N248">
+        <f t="shared" si="1"/>
+        <v>0.94285714285714284</v>
+      </c>
+      <c r="O248">
+        <v>1</v>
+      </c>
+      <c r="P248">
+        <f t="shared" si="2"/>
+        <v>0.94285714285714284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made the graphs more square
</commit_message>
<xml_diff>
--- a/images/AllGraphs.xlsx
+++ b/images/AllGraphs.xlsx
@@ -1364,9 +1364,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11396571595671677"/>
-          <c:y val="3.2497867963600199E-2"/>
-          <c:w val="0.86483616072373881"/>
+          <c:x val="0.19412261882833351"/>
+          <c:y val="4.8434632395652086E-2"/>
+          <c:w val="0.75397771496558208"/>
           <c:h val="0.76176545881358071"/>
         </c:manualLayout>
       </c:layout>
@@ -1405,94 +1405,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>12.8</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.6</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.5</c:v>
+                  <c:v>5.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.9</c:v>
+                  <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.4</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>46.1</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.899999999999999</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41.2</c:v>
+                  <c:v>20.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43.6</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.9</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14.4</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18.899999999999999</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12.3</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13.6</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32.9</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>18.899999999999999</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21.3</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>14</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>24</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>25.9</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.4</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>52.4</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>13.5</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1504,94 +1504,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>3.5</c:v>
+                  <c:v>12.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2</c:v>
+                  <c:v>11.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.2</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0999999999999996</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4</c:v>
+                  <c:v>11.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.3</c:v>
+                  <c:v>11.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5</c:v>
+                  <c:v>46.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>19.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.6</c:v>
+                  <c:v>41.2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25</c:v>
+                  <c:v>43.6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.3</c:v>
+                  <c:v>12.9</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.7</c:v>
+                  <c:v>14.4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.8</c:v>
+                  <c:v>18.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.3</c:v>
+                  <c:v>12.3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.2</c:v>
+                  <c:v>13.6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.5</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.5</c:v>
+                  <c:v>32.9</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>18.899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.4000000000000004</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.5</c:v>
+                  <c:v>21.3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>11</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>16</c:v>
+                  <c:v>25.9</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.2</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>70</c:v>
+                  <c:v>52.4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.3</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1636,20 +1636,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2800">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                  </a:rPr>
-                  <a:t>Call</a:t>
-                </a:r>
-                <a:r>
                   <a:rPr lang="en-US" sz="2800" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t> graph analysis time (sec)</a:t>
+                  <a:t>Call graph size (K)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US" sz="2800">
                   <a:solidFill>
@@ -1659,7 +1651,14 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.33483334488072425"/>
+              <c:y val="0.89087787390527862"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1743,10 +1742,7 @@
                 <a:pPr>
                   <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -1754,13 +1750,19 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2800" baseline="0">
+                  <a:rPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
+                    <a:effectLst/>
                   </a:rPr>
-                  <a:t>Call graph size (K)</a:t>
+                  <a:t>Call graph analysis time (sec)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US" sz="2800" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1768,8 +1770,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="7.6974881489220211E-3"/>
-              <c:y val="0.16993738414086818"/>
+              <c:x val="2.7279991474842041E-2"/>
+              <c:y val="4.9047513458803017E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1787,10 +1789,7 @@
               <a:pPr>
                 <a:defRPr sz="2800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -1900,7 +1899,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18190809630816854"/>
+          <c:y val="4.4179560830695241E-2"/>
+          <c:w val="0.7664331480785268"/>
+          <c:h val="0.72623385677354579"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1912,7 +1921,11 @@
               <a:noFill/>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow>
+                <a:schemeClr val="tx1"/>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
@@ -1926,7 +1939,11 @@
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:glow>
+                  <a:schemeClr val="tx1"/>
+                </a:glow>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
@@ -1936,94 +1953,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.8</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.9</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.1</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.7</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.6</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.6</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.1</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.1</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.5</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.7</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.3</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.9</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.4</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2035,94 +2052,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>42</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>168</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>47</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>207</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8</c:v>
+                  <c:v>3.9</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>39</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>32</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>25</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>31</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>16</c:v>
+                  <c:v>1.4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>13</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2170,7 +2187,7 @@
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Instrumentation Time (sec)</a:t>
+                  <a:t>Units instrumented</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2264,13 +2281,16 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2800" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
+                  <a:rPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
                   </a:rPr>
-                  <a:t>Units instrumented</a:t>
+                  <a:t>Instrumentation Time (sec)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US" sz="2800" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2278,8 +2298,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="8.649935738469533E-3"/>
-              <c:y val="0.15570737973890583"/>
+              <c:x val="1.0791941454835004E-2"/>
+              <c:y val="2.7172882536856919E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2407,7 +2427,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19637676523980283"/>
+          <c:y val="4.4228102089214245E-2"/>
+          <c:w val="0.78246074105352748"/>
+          <c:h val="0.73620999009098476"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -2415,7 +2445,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -2432,7 +2462,9 @@
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
+                  <a:schemeClr val="dk1">
+                    <a:tint val="88500"/>
+                  </a:schemeClr>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -2445,94 +2477,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>3.1</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="15">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2.6</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.1</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2.8</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.3</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>4.4000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.9</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2544,94 +2576,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>25</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>53</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>3.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>11</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>9</c:v>
+                  <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7</c:v>
+                  <c:v>4.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8</c:v>
+                  <c:v>2.9</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2678,7 +2710,7 @@
                       <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Constrint Analysis Time (sec)</a:t>
+                  <a:t>No. of constraints</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2772,13 +2804,16 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2800" b="0" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
+                  <a:rPr lang="en-US" sz="2800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
                   </a:rPr>
-                  <a:t>No. of constraints</a:t>
+                  <a:t>Constrint analysis time (sec)</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US" sz="2800" b="0" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2786,8 +2821,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="6.0199081205597992E-3"/>
-              <c:y val="0.17071696285588794"/>
+              <c:x val="3.113200924993104E-2"/>
+              <c:y val="5.1279020450312573E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -5672,7 +5707,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>212724</xdr:colOff>
+      <xdr:colOff>203200</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
@@ -5680,7 +5715,7 @@
       <xdr:col>21</xdr:col>
       <xdr:colOff>365124</xdr:colOff>
       <xdr:row>94</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5701,16 +5736,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>174877</xdr:colOff>
-      <xdr:row>143</xdr:row>
-      <xdr:rowOff>178189</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>449658</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>119308</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>395850</xdr:colOff>
-      <xdr:row>168</xdr:row>
-      <xdr:rowOff>173181</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5731,16 +5766,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>295068</xdr:colOff>
-      <xdr:row>142</xdr:row>
-      <xdr:rowOff>112850</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>165101</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>22549</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>26643</xdr:colOff>
-      <xdr:row>166</xdr:row>
-      <xdr:rowOff>136663</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>274947</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5761,16 +5796,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>286970</xdr:colOff>
-      <xdr:row>170</xdr:row>
-      <xdr:rowOff>119777</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>193454</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>17316</xdr:colOff>
-      <xdr:row>195</xdr:row>
-      <xdr:rowOff>125752</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>166256</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6057,8 +6092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M127" sqref="M127"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="O167" sqref="O167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6525,242 +6560,242 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
+        <v>3.5</v>
+      </c>
+      <c r="B100">
         <v>12.8</v>
-      </c>
-      <c r="B100">
-        <v>3.5</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
+        <v>3.2</v>
+      </c>
+      <c r="B101">
         <v>11.6</v>
-      </c>
-      <c r="B101">
-        <v>3.2</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
+        <v>3.2</v>
+      </c>
+      <c r="B102">
         <v>12</v>
-      </c>
-      <c r="B102">
-        <v>3.2</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
+        <v>4</v>
+      </c>
+      <c r="B103">
         <v>11.5</v>
-      </c>
-      <c r="B103">
-        <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
+        <v>3.3</v>
+      </c>
+      <c r="B104">
         <v>12</v>
-      </c>
-      <c r="B104">
-        <v>3.3</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B105">
         <v>16.5</v>
-      </c>
-      <c r="B105">
-        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
+        <v>3.4</v>
+      </c>
+      <c r="B106">
         <v>11.9</v>
-      </c>
-      <c r="B106">
-        <v>3.4</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
+        <v>3.3</v>
+      </c>
+      <c r="B107">
         <v>11.4</v>
-      </c>
-      <c r="B107">
-        <v>3.3</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
+        <v>4.5</v>
+      </c>
+      <c r="B108">
         <v>46.1</v>
-      </c>
-      <c r="B108">
-        <v>4.5</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B109">
         <v>19.899999999999999</v>
-      </c>
-      <c r="B109">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
+        <v>20.6</v>
+      </c>
+      <c r="B110">
         <v>41.2</v>
-      </c>
-      <c r="B110">
-        <v>20.6</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
+        <v>25</v>
+      </c>
+      <c r="B111">
         <v>43.6</v>
-      </c>
-      <c r="B111">
-        <v>25</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
+        <v>6.3</v>
+      </c>
+      <c r="B112">
         <v>12.9</v>
-      </c>
-      <c r="B112">
-        <v>6.3</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
+        <v>3.7</v>
+      </c>
+      <c r="B113">
         <v>14.4</v>
-      </c>
-      <c r="B113">
-        <v>3.7</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
+        <v>4.8</v>
+      </c>
+      <c r="B114">
         <v>18.899999999999999</v>
-      </c>
-      <c r="B114">
-        <v>4.8</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B115">
         <v>20</v>
-      </c>
-      <c r="B115">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
+        <v>3.3</v>
+      </c>
+      <c r="B116">
         <v>12.3</v>
-      </c>
-      <c r="B116">
-        <v>3.3</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
+        <v>3.2</v>
+      </c>
+      <c r="B117">
         <v>13.6</v>
-      </c>
-      <c r="B117">
-        <v>3.2</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
+        <v>3.2</v>
+      </c>
+      <c r="B118">
         <v>13</v>
-      </c>
-      <c r="B118">
-        <v>3.2</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
+        <v>4.5</v>
+      </c>
+      <c r="B119">
         <v>17</v>
-      </c>
-      <c r="B119">
-        <v>4.5</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
+        <v>2.5</v>
+      </c>
+      <c r="B120">
         <v>32.9</v>
-      </c>
-      <c r="B120">
-        <v>2.5</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B121">
         <v>18.899999999999999</v>
-      </c>
-      <c r="B121">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B122">
         <v>20</v>
-      </c>
-      <c r="B122">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
+        <v>4.5</v>
+      </c>
+      <c r="B123">
         <v>21.3</v>
-      </c>
-      <c r="B123">
-        <v>4.5</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
+        <v>5</v>
+      </c>
+      <c r="B124">
         <v>14</v>
-      </c>
-      <c r="B124">
-        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
+        <v>11</v>
+      </c>
+      <c r="B125">
         <v>24</v>
-      </c>
-      <c r="B125">
-        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
+        <v>16</v>
+      </c>
+      <c r="B126">
         <v>25.9</v>
-      </c>
-      <c r="B126">
-        <v>16</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
+        <v>6.2</v>
+      </c>
+      <c r="B127">
         <v>2.4</v>
-      </c>
-      <c r="B127">
-        <v>6.2</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
+        <v>70</v>
+      </c>
+      <c r="B128">
         <v>52.4</v>
-      </c>
-      <c r="B128">
-        <v>70</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
+        <v>3.3</v>
+      </c>
+      <c r="B129">
         <v>13.5</v>
-      </c>
-      <c r="B129">
-        <v>3.3</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
@@ -6770,242 +6805,242 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156">
+        <v>42</v>
+      </c>
+      <c r="B156">
         <v>2.2999999999999998</v>
-      </c>
-      <c r="B156">
-        <v>42</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157">
+        <v>19</v>
+      </c>
+      <c r="B157">
         <v>1.9</v>
-      </c>
-      <c r="B157">
-        <v>19</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158">
+        <v>13</v>
+      </c>
+      <c r="B158">
         <v>2</v>
-      </c>
-      <c r="B158">
-        <v>13</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159">
+        <v>46</v>
+      </c>
+      <c r="B159">
         <v>1.8</v>
-      </c>
-      <c r="B159">
-        <v>46</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160">
+        <v>76</v>
+      </c>
+      <c r="B160">
         <v>2</v>
-      </c>
-      <c r="B160">
-        <v>76</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161">
+        <v>168</v>
+      </c>
+      <c r="B161">
         <v>2.8</v>
-      </c>
-      <c r="B161">
-        <v>168</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162">
+        <v>36</v>
+      </c>
+      <c r="B162">
         <v>2.9</v>
-      </c>
-      <c r="B162">
-        <v>36</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163">
+        <v>6</v>
+      </c>
+      <c r="B163">
         <v>1.9</v>
-      </c>
-      <c r="B163">
-        <v>6</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164">
+        <v>20</v>
+      </c>
+      <c r="B164">
         <v>3.1</v>
-      </c>
-      <c r="B164">
-        <v>20</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165">
+        <v>47</v>
+      </c>
+      <c r="B165">
         <v>2.7</v>
-      </c>
-      <c r="B165">
-        <v>47</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166">
+        <v>4</v>
+      </c>
+      <c r="B166">
         <v>1.6</v>
-      </c>
-      <c r="B166">
-        <v>4</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167">
+        <v>6</v>
+      </c>
+      <c r="B167">
         <v>1.6</v>
-      </c>
-      <c r="B167">
-        <v>6</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168">
+        <v>207</v>
+      </c>
+      <c r="B168">
         <v>2.6</v>
-      </c>
-      <c r="B168">
-        <v>207</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169">
+        <v>28</v>
+      </c>
+      <c r="B169">
         <v>3.1</v>
-      </c>
-      <c r="B169">
-        <v>28</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170">
+        <v>13</v>
+      </c>
+      <c r="B170">
         <v>3.1</v>
-      </c>
-      <c r="B170">
-        <v>13</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171">
+        <v>8</v>
+      </c>
+      <c r="B171">
         <v>1.6</v>
-      </c>
-      <c r="B171">
-        <v>8</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172">
+        <v>6</v>
+      </c>
+      <c r="B172">
         <v>2.7</v>
-      </c>
-      <c r="B172">
-        <v>6</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173">
+        <v>10</v>
+      </c>
+      <c r="B173">
         <v>2.9</v>
-      </c>
-      <c r="B173">
-        <v>10</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174">
+        <v>6</v>
+      </c>
+      <c r="B174">
         <v>2.5</v>
-      </c>
-      <c r="B174">
-        <v>6</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175">
+        <v>4</v>
+      </c>
+      <c r="B175">
         <v>1.6</v>
-      </c>
-      <c r="B175">
-        <v>4</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176">
+        <v>8</v>
+      </c>
+      <c r="B176">
         <v>3.9</v>
-      </c>
-      <c r="B176">
-        <v>8</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177">
+        <v>6</v>
+      </c>
+      <c r="B177">
         <v>2.8</v>
-      </c>
-      <c r="B177">
-        <v>6</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178">
+        <v>8</v>
+      </c>
+      <c r="B178">
         <v>2.6</v>
-      </c>
-      <c r="B178">
-        <v>8</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179">
+        <v>39</v>
+      </c>
+      <c r="B179">
         <v>3.5</v>
-      </c>
-      <c r="B179">
-        <v>39</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180">
+        <v>32</v>
+      </c>
+      <c r="B180">
         <v>2.2999999999999998</v>
-      </c>
-      <c r="B180">
-        <v>32</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181">
+        <v>25</v>
+      </c>
+      <c r="B181">
         <v>2.7</v>
-      </c>
-      <c r="B181">
-        <v>25</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182">
+        <v>25</v>
+      </c>
+      <c r="B182">
         <v>1.3</v>
-      </c>
-      <c r="B182">
-        <v>25</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183">
+        <v>31</v>
+      </c>
+      <c r="B183">
         <v>1.9</v>
-      </c>
-      <c r="B183">
-        <v>31</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184">
+        <v>16</v>
+      </c>
+      <c r="B184">
         <v>1.4</v>
-      </c>
-      <c r="B184">
-        <v>16</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185">
+        <v>13</v>
+      </c>
+      <c r="B185">
         <v>2.2000000000000002</v>
-      </c>
-      <c r="B185">
-        <v>13</v>
       </c>
     </row>
     <row r="210" spans="1:16" x14ac:dyDescent="0.25">
@@ -7015,12 +7050,12 @@
     </row>
     <row r="211" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A211">
-        <v>3.1</v>
-      </c>
-      <c r="B211">
         <f>FLOOR((C211-D211)/3,1)</f>
         <v>12</v>
       </c>
+      <c r="B211">
+        <v>3.1</v>
+      </c>
       <c r="C211">
         <v>42</v>
       </c>
@@ -7030,11 +7065,11 @@
     </row>
     <row r="212" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A212">
+        <f>FLOOR((C212-D212)/3,1)</f>
+        <v>0</v>
+      </c>
+      <c r="B212">
         <v>2.8</v>
-      </c>
-      <c r="B212">
-        <f t="shared" ref="B212:B240" si="0">FLOOR((C212-D212)/3,1)</f>
-        <v>0</v>
       </c>
       <c r="C212">
         <v>19</v>
@@ -7045,11 +7080,11 @@
     </row>
     <row r="213" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A213">
+        <f>FLOOR((C213-D213)/3,1)</f>
+        <v>3</v>
+      </c>
+      <c r="B213">
         <v>2.8</v>
-      </c>
-      <c r="B213">
-        <f t="shared" si="0"/>
-        <v>3</v>
       </c>
       <c r="C213">
         <v>13</v>
@@ -7060,11 +7095,11 @@
     </row>
     <row r="214" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A214">
+        <f>FLOOR((C214-D214)/3,1)</f>
+        <v>14</v>
+      </c>
+      <c r="B214">
         <v>2.7</v>
-      </c>
-      <c r="B214">
-        <f t="shared" si="0"/>
-        <v>14</v>
       </c>
       <c r="C214">
         <v>46</v>
@@ -7075,11 +7110,11 @@
     </row>
     <row r="215" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A215">
+        <f>FLOOR((C215-D215)/3,1)</f>
+        <v>25</v>
+      </c>
+      <c r="B215">
         <v>3</v>
-      </c>
-      <c r="B215">
-        <f t="shared" si="0"/>
-        <v>25</v>
       </c>
       <c r="C215">
         <v>76</v>
@@ -7090,11 +7125,11 @@
     </row>
     <row r="216" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A216">
+        <f>FLOOR((C216-D216)/3,1)</f>
+        <v>53</v>
+      </c>
+      <c r="B216">
         <v>3</v>
-      </c>
-      <c r="B216">
-        <f t="shared" si="0"/>
-        <v>53</v>
       </c>
       <c r="C216">
         <v>168</v>
@@ -7105,11 +7140,11 @@
     </row>
     <row r="217" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A217">
+        <f>FLOOR((C217-D217)/3,1)</f>
+        <v>11</v>
+      </c>
+      <c r="B217">
         <v>3</v>
-      </c>
-      <c r="B217">
-        <f t="shared" si="0"/>
-        <v>11</v>
       </c>
       <c r="C217">
         <v>36</v>
@@ -7132,11 +7167,11 @@
     </row>
     <row r="218" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A218">
+        <f>FLOOR((C218-D218)/3,1)</f>
+        <v>1</v>
+      </c>
+      <c r="B218">
         <v>2.8</v>
-      </c>
-      <c r="B218">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
       <c r="C218">
         <v>6</v>
@@ -7165,11 +7200,11 @@
     </row>
     <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219">
+        <f>FLOOR((C219-D219)/3,1)</f>
+        <v>6</v>
+      </c>
+      <c r="B219">
         <v>3.7</v>
-      </c>
-      <c r="B219">
-        <f t="shared" si="0"/>
-        <v>6</v>
       </c>
       <c r="C219">
         <v>20</v>
@@ -7200,11 +7235,11 @@
     </row>
     <row r="220" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A220">
+        <f>FLOOR((C220-D220)/3,1)</f>
+        <v>13</v>
+      </c>
+      <c r="B220">
         <v>3.3</v>
-      </c>
-      <c r="B220">
-        <f t="shared" si="0"/>
-        <v>13</v>
       </c>
       <c r="C220">
         <v>47</v>
@@ -7222,7 +7257,7 @@
         <v>4</v>
       </c>
       <c r="N220">
-        <f t="shared" ref="N220:N248" si="1">(K220+M220)/(K220+L220)</f>
+        <f t="shared" ref="N220:N248" si="0">(K220+M220)/(K220+L220)</f>
         <v>0.79166666666666663</v>
       </c>
       <c r="O220">
@@ -7235,186 +7270,186 @@
     </row>
     <row r="221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A221">
+        <f>FLOOR((C221-D221)/3,1)</f>
+        <v>1</v>
+      </c>
+      <c r="B221">
         <v>3.1</v>
       </c>
-      <c r="B221">
+      <c r="C221">
+        <v>4</v>
+      </c>
+      <c r="D221">
+        <v>1</v>
+      </c>
+      <c r="K221">
+        <v>21</v>
+      </c>
+      <c r="L221">
+        <v>2</v>
+      </c>
+      <c r="M221">
+        <v>2</v>
+      </c>
+      <c r="N221">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C221">
+      <c r="O221">
+        <v>0.5</v>
+      </c>
+      <c r="P221">
+        <f t="shared" ref="P220:P248" si="1" xml:space="preserve"> N221 * O221</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <f>FLOOR((C222-D222)/3,1)</f>
+        <v>1</v>
+      </c>
+      <c r="B222">
+        <v>3.8</v>
+      </c>
+      <c r="C222">
+        <v>6</v>
+      </c>
+      <c r="D222">
+        <v>1</v>
+      </c>
+      <c r="K222">
+        <v>134</v>
+      </c>
+      <c r="L222">
         <v>4</v>
       </c>
-      <c r="D221">
+      <c r="M222">
+        <v>3</v>
+      </c>
+      <c r="N222">
+        <f t="shared" si="0"/>
+        <v>0.99275362318840576</v>
+      </c>
+      <c r="O222">
         <v>1</v>
       </c>
-      <c r="K221">
-        <v>21</v>
-      </c>
-      <c r="L221">
+      <c r="P222">
+        <f t="shared" si="1"/>
+        <v>0.99275362318840576</v>
+      </c>
+    </row>
+    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <f>FLOOR((C223-D223)/3,1)</f>
+        <v>60</v>
+      </c>
+      <c r="B223">
+        <v>4.8</v>
+      </c>
+      <c r="C223">
+        <v>207</v>
+      </c>
+      <c r="D223">
+        <v>25</v>
+      </c>
+      <c r="K223">
+        <v>125</v>
+      </c>
+      <c r="L223">
+        <v>1</v>
+      </c>
+      <c r="M223">
+        <v>3</v>
+      </c>
+      <c r="N223">
+        <f t="shared" si="0"/>
+        <v>1.0158730158730158</v>
+      </c>
+      <c r="O223">
+        <v>1</v>
+      </c>
+      <c r="P223">
+        <f t="shared" si="1"/>
+        <v>1.0158730158730158</v>
+      </c>
+    </row>
+    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <f>FLOOR((C224-D224)/3,1)</f>
+        <v>7</v>
+      </c>
+      <c r="B224">
+        <v>2.6</v>
+      </c>
+      <c r="C224">
+        <v>28</v>
+      </c>
+      <c r="D224">
+        <v>5</v>
+      </c>
+      <c r="K224">
+        <v>240</v>
+      </c>
+      <c r="L224">
+        <v>8</v>
+      </c>
+      <c r="M224">
+        <v>4</v>
+      </c>
+      <c r="N224">
+        <f t="shared" si="0"/>
+        <v>0.9838709677419355</v>
+      </c>
+      <c r="O224">
+        <v>1</v>
+      </c>
+      <c r="P224">
+        <f t="shared" si="1"/>
+        <v>0.9838709677419355</v>
+      </c>
+    </row>
+    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <f>FLOOR((C225-D225)/3,1)</f>
+        <v>3</v>
+      </c>
+      <c r="B225">
+        <v>3.2</v>
+      </c>
+      <c r="C225">
+        <v>13</v>
+      </c>
+      <c r="D225">
         <v>2</v>
       </c>
-      <c r="M221">
+      <c r="K225">
+        <v>300</v>
+      </c>
+      <c r="L225">
         <v>2</v>
       </c>
-      <c r="N221">
+      <c r="M225">
+        <v>2</v>
+      </c>
+      <c r="N225">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O225">
+        <v>1</v>
+      </c>
+      <c r="P225">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="O221">
-        <v>0.5</v>
-      </c>
-      <c r="P221">
-        <f t="shared" ref="P220:P248" si="2" xml:space="preserve"> N221 * O221</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A222">
-        <v>3.8</v>
-      </c>
-      <c r="B222">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C222">
-        <v>6</v>
-      </c>
-      <c r="D222">
-        <v>1</v>
-      </c>
-      <c r="K222">
-        <v>134</v>
-      </c>
-      <c r="L222">
-        <v>4</v>
-      </c>
-      <c r="M222">
-        <v>3</v>
-      </c>
-      <c r="N222">
-        <f t="shared" si="1"/>
-        <v>0.99275362318840576</v>
-      </c>
-      <c r="O222">
-        <v>1</v>
-      </c>
-      <c r="P222">
-        <f t="shared" si="2"/>
-        <v>0.99275362318840576</v>
-      </c>
-    </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A223">
-        <v>4.8</v>
-      </c>
-      <c r="B223">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="C223">
-        <v>207</v>
-      </c>
-      <c r="D223">
-        <v>25</v>
-      </c>
-      <c r="K223">
-        <v>125</v>
-      </c>
-      <c r="L223">
-        <v>1</v>
-      </c>
-      <c r="M223">
-        <v>3</v>
-      </c>
-      <c r="N223">
-        <f t="shared" si="1"/>
-        <v>1.0158730158730158</v>
-      </c>
-      <c r="O223">
-        <v>1</v>
-      </c>
-      <c r="P223">
-        <f t="shared" si="2"/>
-        <v>1.0158730158730158</v>
-      </c>
-    </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A224">
-        <v>2.6</v>
-      </c>
-      <c r="B224">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C224">
-        <v>28</v>
-      </c>
-      <c r="D224">
-        <v>5</v>
-      </c>
-      <c r="K224">
-        <v>240</v>
-      </c>
-      <c r="L224">
-        <v>8</v>
-      </c>
-      <c r="M224">
-        <v>4</v>
-      </c>
-      <c r="N224">
-        <f t="shared" si="1"/>
-        <v>0.9838709677419355</v>
-      </c>
-      <c r="O224">
-        <v>1</v>
-      </c>
-      <c r="P224">
-        <f t="shared" si="2"/>
-        <v>0.9838709677419355</v>
-      </c>
-    </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A225">
-        <v>3.2</v>
-      </c>
-      <c r="B225">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C225">
-        <v>13</v>
-      </c>
-      <c r="D225">
-        <v>2</v>
-      </c>
-      <c r="K225">
-        <v>300</v>
-      </c>
-      <c r="L225">
-        <v>2</v>
-      </c>
-      <c r="M225">
-        <v>2</v>
-      </c>
-      <c r="N225">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="O225">
-        <v>1</v>
-      </c>
-      <c r="P225">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="226" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A226">
+        <f>FLOOR((C226-D226)/3,1)</f>
+        <v>2</v>
+      </c>
+      <c r="B226">
         <v>3.4</v>
-      </c>
-      <c r="B226">
-        <f t="shared" si="0"/>
-        <v>2</v>
       </c>
       <c r="C226">
         <v>8</v>
@@ -7432,7 +7467,7 @@
         <v>2</v>
       </c>
       <c r="N226">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.0666666666666667</v>
       </c>
       <c r="O226">
@@ -7445,46 +7480,46 @@
     </row>
     <row r="227" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A227">
+        <f>FLOOR((C227-D227)/3,1)</f>
+        <v>1</v>
+      </c>
+      <c r="B227">
         <v>2.8</v>
       </c>
-      <c r="B227">
+      <c r="C227">
+        <v>6</v>
+      </c>
+      <c r="D227">
+        <v>1</v>
+      </c>
+      <c r="K227">
+        <v>37</v>
+      </c>
+      <c r="L227">
+        <v>2</v>
+      </c>
+      <c r="M227">
+        <v>2</v>
+      </c>
+      <c r="N227">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="C227">
-        <v>6</v>
-      </c>
-      <c r="D227">
+      <c r="O227">
         <v>1</v>
       </c>
-      <c r="K227">
-        <v>37</v>
-      </c>
-      <c r="L227">
-        <v>2</v>
-      </c>
-      <c r="M227">
-        <v>2</v>
-      </c>
-      <c r="N227">
+      <c r="P227">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="O227">
-        <v>1</v>
-      </c>
-      <c r="P227">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="228" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A228">
+        <f>FLOOR((C228-D228)/3,1)</f>
+        <v>2</v>
+      </c>
+      <c r="B228">
         <v>3.1</v>
-      </c>
-      <c r="B228">
-        <f t="shared" si="0"/>
-        <v>2</v>
       </c>
       <c r="C228">
         <v>10</v>
@@ -7502,7 +7537,7 @@
         <v>4</v>
       </c>
       <c r="N228">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.95652173913043481</v>
       </c>
       <c r="O228">
@@ -7515,11 +7550,11 @@
     </row>
     <row r="229" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A229">
+        <f>FLOOR((C229-D229)/3,1)</f>
+        <v>1</v>
+      </c>
+      <c r="B229">
         <v>2.8</v>
-      </c>
-      <c r="B229">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
       <c r="C229">
         <v>6</v>
@@ -7537,23 +7572,23 @@
         <v>3</v>
       </c>
       <c r="N229">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.0392156862745099</v>
       </c>
       <c r="O229">
         <v>0.5</v>
       </c>
       <c r="P229">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.51960784313725494</v>
       </c>
     </row>
     <row r="230" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A230">
+        <v>1</v>
+      </c>
+      <c r="B230">
         <v>3.8</v>
-      </c>
-      <c r="B230">
-        <v>1</v>
       </c>
       <c r="C230">
         <v>4</v>
@@ -7571,24 +7606,24 @@
         <v>2</v>
       </c>
       <c r="N230">
+        <f t="shared" si="0"/>
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="O230">
+        <v>1</v>
+      </c>
+      <c r="P230">
         <f t="shared" si="1"/>
         <v>1.0249999999999999</v>
       </c>
-      <c r="O230">
-        <v>1</v>
-      </c>
-      <c r="P230">
-        <f t="shared" si="2"/>
-        <v>1.0249999999999999</v>
-      </c>
     </row>
     <row r="231" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A231">
+        <f>FLOOR((C231-D231)/3,1)</f>
+        <v>2</v>
+      </c>
+      <c r="B231">
         <v>3.2</v>
-      </c>
-      <c r="B231">
-        <f t="shared" si="0"/>
-        <v>2</v>
       </c>
       <c r="C231">
         <v>8</v>
@@ -7606,24 +7641,24 @@
         <v>0</v>
       </c>
       <c r="N231">
+        <f t="shared" si="0"/>
+        <v>0.96</v>
+      </c>
+      <c r="O231">
+        <v>1</v>
+      </c>
+      <c r="P231">
         <f t="shared" si="1"/>
         <v>0.96</v>
       </c>
-      <c r="O231">
-        <v>1</v>
-      </c>
-      <c r="P231">
-        <f t="shared" si="2"/>
-        <v>0.96</v>
-      </c>
     </row>
     <row r="232" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A232">
+        <f>FLOOR((C232-D232)/3,1)</f>
+        <v>1</v>
+      </c>
+      <c r="B232">
         <v>3.1</v>
-      </c>
-      <c r="B232">
-        <f t="shared" si="0"/>
-        <v>1</v>
       </c>
       <c r="C232">
         <v>6</v>
@@ -7641,24 +7676,24 @@
         <v>20</v>
       </c>
       <c r="N232">
+        <f t="shared" si="0"/>
+        <v>1.375</v>
+      </c>
+      <c r="O232">
+        <v>1</v>
+      </c>
+      <c r="P232">
         <f t="shared" si="1"/>
         <v>1.375</v>
       </c>
-      <c r="O232">
-        <v>1</v>
-      </c>
-      <c r="P232">
-        <f t="shared" si="2"/>
-        <v>1.375</v>
-      </c>
     </row>
     <row r="233" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A233">
+        <f>FLOOR((C233-D233)/3,1)</f>
+        <v>2</v>
+      </c>
+      <c r="B233">
         <v>3.3</v>
-      </c>
-      <c r="B233">
-        <f t="shared" si="0"/>
-        <v>2</v>
       </c>
       <c r="C233">
         <v>8</v>
@@ -7676,24 +7711,24 @@
         <v>3</v>
       </c>
       <c r="N233">
+        <f t="shared" si="0"/>
+        <v>1.0158730158730158</v>
+      </c>
+      <c r="O233">
+        <v>1</v>
+      </c>
+      <c r="P233">
         <f t="shared" si="1"/>
         <v>1.0158730158730158</v>
       </c>
-      <c r="O233">
-        <v>1</v>
-      </c>
-      <c r="P233">
-        <f t="shared" si="2"/>
-        <v>1.0158730158730158</v>
-      </c>
     </row>
     <row r="234" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A234">
+        <f>FLOOR((C234-D234)/3,1)</f>
+        <v>11</v>
+      </c>
+      <c r="B234">
         <v>3</v>
-      </c>
-      <c r="B234">
-        <f t="shared" si="0"/>
-        <v>11</v>
       </c>
       <c r="C234">
         <v>39</v>
@@ -7711,7 +7746,7 @@
         <v>4</v>
       </c>
       <c r="N234">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.125</v>
       </c>
       <c r="O234">
@@ -7724,11 +7759,11 @@
     </row>
     <row r="235" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A235">
+        <f>FLOOR((C235-D235)/3,1)</f>
+        <v>9</v>
+      </c>
+      <c r="B235">
         <v>3.4</v>
-      </c>
-      <c r="B235">
-        <f t="shared" si="0"/>
-        <v>9</v>
       </c>
       <c r="C235">
         <v>32</v>
@@ -7746,7 +7781,7 @@
         <v>3</v>
       </c>
       <c r="N235">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.1333333333333333</v>
       </c>
       <c r="O235">
@@ -7759,11 +7794,11 @@
     </row>
     <row r="236" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A236">
+        <f>FLOOR((C236-D236)/3,1)</f>
+        <v>7</v>
+      </c>
+      <c r="B236">
         <v>4.4000000000000004</v>
-      </c>
-      <c r="B236">
-        <f t="shared" si="0"/>
-        <v>7</v>
       </c>
       <c r="C236">
         <v>25</v>
@@ -7781,24 +7816,24 @@
         <v>0</v>
       </c>
       <c r="N236">
+        <f t="shared" si="0"/>
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="O236">
+        <v>1</v>
+      </c>
+      <c r="P236">
         <f t="shared" si="1"/>
         <v>0.97222222222222221</v>
       </c>
-      <c r="O236">
-        <v>1</v>
-      </c>
-      <c r="P236">
-        <f t="shared" si="2"/>
-        <v>0.97222222222222221</v>
-      </c>
     </row>
     <row r="237" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A237">
+        <f>FLOOR((C237-D237)/3,1)</f>
+        <v>7</v>
+      </c>
+      <c r="B237">
         <v>3</v>
-      </c>
-      <c r="B237">
-        <f t="shared" si="0"/>
-        <v>7</v>
       </c>
       <c r="C237">
         <v>25</v>
@@ -7816,24 +7851,24 @@
         <v>1</v>
       </c>
       <c r="N237">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O237">
+        <v>1</v>
+      </c>
+      <c r="P237">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="O237">
-        <v>1</v>
-      </c>
-      <c r="P237">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="238" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A238">
+        <f>FLOOR((C238-D238)/3,1)</f>
+        <v>8</v>
+      </c>
+      <c r="B238">
         <v>2.9</v>
-      </c>
-      <c r="B238">
-        <f t="shared" si="0"/>
-        <v>8</v>
       </c>
       <c r="C238">
         <v>31</v>
@@ -7851,24 +7886,24 @@
         <v>1</v>
       </c>
       <c r="N238">
+        <f t="shared" si="0"/>
+        <v>0.98076923076923073</v>
+      </c>
+      <c r="O238">
+        <v>1</v>
+      </c>
+      <c r="P238">
         <f t="shared" si="1"/>
         <v>0.98076923076923073</v>
       </c>
-      <c r="O238">
-        <v>1</v>
-      </c>
-      <c r="P238">
-        <f t="shared" si="2"/>
-        <v>0.98076923076923073</v>
-      </c>
     </row>
     <row r="239" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A239">
+        <f>FLOOR((C239-D239)/3,1)</f>
+        <v>5</v>
+      </c>
+      <c r="B239">
         <v>3</v>
-      </c>
-      <c r="B239">
-        <f t="shared" si="0"/>
-        <v>5</v>
       </c>
       <c r="C239">
         <v>16</v>
@@ -7886,24 +7921,24 @@
         <v>2</v>
       </c>
       <c r="N239">
+        <f t="shared" si="0"/>
+        <v>1.0109890109890109</v>
+      </c>
+      <c r="O239">
+        <v>1</v>
+      </c>
+      <c r="P239">
         <f t="shared" si="1"/>
         <v>1.0109890109890109</v>
       </c>
-      <c r="O239">
-        <v>1</v>
-      </c>
-      <c r="P239">
-        <f t="shared" si="2"/>
-        <v>1.0109890109890109</v>
-      </c>
     </row>
     <row r="240" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A240">
+        <f>FLOOR((C240-D240)/3,1)</f>
+        <v>3</v>
+      </c>
+      <c r="B240">
         <v>2.7</v>
-      </c>
-      <c r="B240">
-        <f t="shared" si="0"/>
-        <v>3</v>
       </c>
       <c r="C240">
         <v>13</v>
@@ -7921,14 +7956,14 @@
         <v>5</v>
       </c>
       <c r="N240">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.1379310344827587</v>
       </c>
       <c r="O240">
         <v>1</v>
       </c>
       <c r="P240">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.1379310344827587</v>
       </c>
     </row>
@@ -7943,7 +7978,7 @@
         <v>1</v>
       </c>
       <c r="N241">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O241">
@@ -7965,14 +8000,14 @@
         <v>4</v>
       </c>
       <c r="N242">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.96875</v>
       </c>
       <c r="O242">
         <v>1</v>
       </c>
       <c r="P242">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.96875</v>
       </c>
     </row>
@@ -7987,7 +8022,7 @@
         <v>1</v>
       </c>
       <c r="N243">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.97647058823529409</v>
       </c>
       <c r="O243">
@@ -8009,14 +8044,14 @@
         <v>9</v>
       </c>
       <c r="N244">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.0245098039215685</v>
       </c>
       <c r="O244">
         <v>1</v>
       </c>
       <c r="P244">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.0245098039215685</v>
       </c>
     </row>
@@ -8031,14 +8066,14 @@
         <v>0</v>
       </c>
       <c r="N245">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.97560975609756095</v>
       </c>
       <c r="O245">
         <v>1</v>
       </c>
       <c r="P245">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.97560975609756095</v>
       </c>
     </row>
@@ -8053,14 +8088,14 @@
         <v>2</v>
       </c>
       <c r="N246">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.96052631578947367</v>
       </c>
       <c r="O246">
         <v>1</v>
       </c>
       <c r="P246">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.96052631578947367</v>
       </c>
     </row>
@@ -8075,7 +8110,7 @@
         <v>3</v>
       </c>
       <c r="N247">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.0289855072463767</v>
       </c>
       <c r="O247">
@@ -8097,14 +8132,14 @@
         <v>0</v>
       </c>
       <c r="N248">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.94285714285714284</v>
       </c>
       <c r="O248">
         <v>1</v>
       </c>
       <c r="P248">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.94285714285714284</v>
       </c>
     </row>
@@ -8118,7 +8153,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B100:B130">
+  <conditionalFormatting sqref="A100:A129 B130">
     <cfRule type="iconSet" priority="2">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
@@ -8127,7 +8162,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A100:A130">
+  <conditionalFormatting sqref="B100:B129 A130">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>

</xml_diff>